<commit_message>
created objects for each item, need to continue adding to mine attributes excel file
</commit_message>
<xml_diff>
--- a/data/mine_attributes.xlsx
+++ b/data/mine_attributes.xlsx
@@ -8,16 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/Documents/University Work/summer internship/pycharm_factory/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27875321-83AD-0140-9AC1-42CA85ED7EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08CF534B-B80A-524F-8E12-5BACC1F96386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34720" yWindow="-320" windowWidth="26480" windowHeight="16220" xr2:uid="{E883CBF3-2CDB-0D4C-B75C-CDFD4FA8C312}"/>
+    <workbookView xWindow="37320" yWindow="-900" windowWidth="28040" windowHeight="16940" activeTab="5" xr2:uid="{E883CBF3-2CDB-0D4C-B75C-CDFD4FA8C312}"/>
   </bookViews>
   <sheets>
     <sheet name="macro details" sheetId="8" r:id="rId1"/>
-    <sheet name="continuous miner" sheetId="4" r:id="rId2"/>
-    <sheet name="roof bolter" sheetId="6" r:id="rId3"/>
-    <sheet name="shuttle car" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId5"/>
+    <sheet name="utility" sheetId="10" r:id="rId2"/>
+    <sheet name="continuous miner" sheetId="4" r:id="rId3"/>
+    <sheet name="roof bolter" sheetId="6" r:id="rId4"/>
+    <sheet name="longwall shearer" sheetId="11" r:id="rId5"/>
+    <sheet name="LHD" sheetId="12" r:id="rId6"/>
+    <sheet name="shuttle car" sheetId="5" r:id="rId7"/>
+    <sheet name="worker" sheetId="9" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="61">
   <si>
     <t xml:space="preserve">company </t>
   </si>
@@ -100,12 +104,6 @@
     <t>longwall miner</t>
   </si>
   <si>
-    <t xml:space="preserve">production output </t>
-  </si>
-  <si>
-    <t>maintenace hrs per week</t>
-  </si>
-  <si>
     <t>key</t>
   </si>
   <si>
@@ -118,18 +116,15 @@
     <t>hrs</t>
   </si>
   <si>
-    <t>usage per week</t>
-  </si>
-  <si>
     <t>nameplate rating</t>
   </si>
   <si>
-    <t>worker</t>
-  </si>
-  <si>
     <t>10sc32B</t>
   </si>
   <si>
+    <t>model</t>
+  </si>
+  <si>
     <t xml:space="preserve">units </t>
   </si>
   <si>
@@ -145,18 +140,12 @@
     <t>power</t>
   </si>
   <si>
-    <t xml:space="preserve">power </t>
-  </si>
-  <si>
     <t>14CM15D</t>
   </si>
   <si>
     <t>joy quadbolter</t>
   </si>
   <si>
-    <t>maintenace per week</t>
-  </si>
-  <si>
     <t>proven + probable deposits</t>
   </si>
   <si>
@@ -173,6 +162,69 @@
   </si>
   <si>
     <t xml:space="preserve">tonnes </t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>Green River, WY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value </t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>wage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$/yr </t>
+  </si>
+  <si>
+    <t>ore market price</t>
+  </si>
+  <si>
+    <t>$/tonne</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>fuel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">electricity </t>
+  </si>
+  <si>
+    <t>ore density</t>
+  </si>
+  <si>
+    <t>g/cm3</t>
+  </si>
+  <si>
+    <t>hrs/wk</t>
+  </si>
+  <si>
+    <t>usage</t>
+  </si>
+  <si>
+    <t>production output</t>
+  </si>
+  <si>
+    <t>maintenance</t>
+  </si>
+  <si>
+    <t>workers</t>
+  </si>
+  <si>
+    <t>shift length</t>
+  </si>
+  <si>
+    <t>depth</t>
+  </si>
+  <si>
+    <t>m</t>
   </si>
 </sst>
 </file>
@@ -527,59 +579,143 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ABFB296-438E-1747-ABC9-555CDE54E2A4}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A2:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" t="s">
-        <v>30</v>
-      </c>
-    </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2">
-        <v>5000000</v>
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B3">
-        <v>234</v>
+        <v>5000000</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4">
+        <v>475</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5">
+        <v>234</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6">
+        <v>0.9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7">
+        <v>2.13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>40</v>
       </c>
-      <c r="B4">
-        <v>0.9</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B8" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9">
+        <v>250</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F27F4F09-9562-8F4C-A40E-927BF5DC3D04}">
+  <dimension ref="A2:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -587,12 +723,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F6C306B-8A58-6F47-B920-204089AE08B3}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -602,69 +738,77 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
         <v>22</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3">
-        <v>139</v>
-      </c>
-      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="B4">
-        <v>110</v>
+        <v>139</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="B5">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="B6">
-        <v>600</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B7">
+        <v>600</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8">
         <v>2</v>
       </c>
     </row>
@@ -673,12 +817,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62385A2F-9BCF-E84D-987B-70F09662E5AB}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -688,58 +832,66 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
         <v>22</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>26</v>
       </c>
-      <c r="B3">
-        <v>110</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
+      <c r="B3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="B4">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="B5">
-        <v>125</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B6">
+        <v>125</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7">
         <v>3</v>
       </c>
     </row>
@@ -748,12 +900,40 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C99E2633-F0B0-0F4F-8FA5-326C9D7CE73B}">
-  <dimension ref="A1:C7"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6659977-9172-CD46-8451-C5DE37D17549}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{231CCEC4-3D3D-4143-AE0F-E82354A19379}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C99E2633-F0B0-0F4F-8FA5-326C9D7CE73B}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -763,69 +943,77 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>31</v>
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B4">
-        <v>110</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="B5">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="B6">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B7">
+        <v>85</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8">
         <v>1</v>
       </c>
     </row>
@@ -834,7 +1022,55 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA6ED9ED-AFC7-5E4D-A019-3E513DE76C3A}">
+  <dimension ref="A2:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3">
+        <v>70000</v>
+      </c>
+      <c r="C3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{318DF2EB-565B-D749-9801-BCC60DA85E15}">
   <dimension ref="B2:I6"/>
   <sheetViews>

</xml_diff>